<commit_message>
Calculation of Confidence intervals, with unknown Population Varience using t-score
</commit_message>
<xml_diff>
--- a/4_2_population-variance-known-z-score-exercise.xlsx
+++ b/4_2_population-variance-known-z-score-exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Stuff\Documents\EPITA\365 Data Science\Statistics-for-data-science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6AA394-C9AF-402C-8193-E6310BBCB00F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A60F3E9-CA20-42E2-AA79-4FD443C907C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Data scientist salary</t>
   </si>
@@ -66,16 +66,22 @@
     <t>Standard Error</t>
   </si>
   <si>
-    <t>confidence of 99% impplies a = 0.01</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-0.001 = </t>
-  </si>
-  <si>
-    <t>Za = 2.5 + 0.08</t>
+    <t>confidence of 99% impplies a = 1/100</t>
+  </si>
+  <si>
+    <t>a = 0.01</t>
+  </si>
+  <si>
+    <t>Z/2  = 0.01/2</t>
+  </si>
+  <si>
+    <t>1-0.005</t>
+  </si>
+  <si>
+    <t>Z0.005 = 0.995</t>
+  </si>
+  <si>
+    <t>Za = 2.5+0.07</t>
   </si>
 </sst>
 </file>
@@ -523,7 +529,7 @@
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -641,7 +647,9 @@
       <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="10"/>
@@ -656,10 +664,10 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="12">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -674,7 +682,7 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E16" s="12">
         <v>0.995</v>
@@ -692,8 +700,12 @@
         <v>80740</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.05</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -721,10 +733,10 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19" s="8">
-        <v>2.58</v>
+        <v>2.57</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -755,11 +767,11 @@
       <c r="D21" s="8"/>
       <c r="E21" s="15">
         <f>$E$12-($E$19*$E$13)</f>
-        <v>93134.745674850026</v>
+        <v>93162.131802725286</v>
       </c>
       <c r="F21" s="15">
         <f>$E$12+($E$19*$E$13)</f>
-        <v>107265.98765848331</v>
+        <v>107238.60153060805</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>

</xml_diff>